<commit_message>
refacto to be able to move xls specific
</commit_message>
<xml_diff>
--- a/nodejs/src/jira-report-js-full.xlsx
+++ b/nodejs/src/jira-report-js-full.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="910">
   <si>
     <t>Raw metrics</t>
   </si>
@@ -220,6 +220,18 @@
     <t>2020-7-15</t>
   </si>
   <si>
+    <t>TDC Sprint 41</t>
+  </si>
+  <si>
+    <t>2020-8-25 00:30</t>
+  </si>
+  <si>
+    <t>2020-9-10 14:54</t>
+  </si>
+  <si>
+    <t>2020-9-10 13:31</t>
+  </si>
+  <si>
     <t>TDC-4121</t>
   </si>
   <si>
@@ -253,7 +265,7 @@
     <t>2020-7-17</t>
   </si>
   <si>
-    <t>TDC Sprint 41</t>
+    <t>TDC Sprint 42</t>
   </si>
   <si>
     <t>TDC-4479</t>
@@ -283,7 +295,7 @@
     <t>TDC-4501</t>
   </si>
   <si>
-    <t>TDC Sprint 42</t>
+    <t>TDC Sprint 43</t>
   </si>
   <si>
     <t>TDC-4552</t>
@@ -310,7 +322,7 @@
     <t>2020-7-20</t>
   </si>
   <si>
-    <t>TDC Sprint 43</t>
+    <t>TDC Sprint 44</t>
   </si>
   <si>
     <t>TDC-4481</t>
@@ -340,7 +352,7 @@
     <t>TDC-4226</t>
   </si>
   <si>
-    <t>TDC Sprint 44</t>
+    <t>TDC Sprint 45</t>
   </si>
   <si>
     <t>TDC-4081</t>
@@ -385,7 +397,7 @@
     <t>2020-7-21</t>
   </si>
   <si>
-    <t>TDC Sprint 45</t>
+    <t>TDC Sprint 46</t>
   </si>
   <si>
     <t>TDC-4551</t>
@@ -406,7 +418,7 @@
     <t>2020-7-24</t>
   </si>
   <si>
-    <t>TDC Sprint 46</t>
+    <t>TDC Sprint 47</t>
   </si>
   <si>
     <t>TDC-4642</t>
@@ -445,7 +457,7 @@
     <t>TDC-4535</t>
   </si>
   <si>
-    <t>TDC Sprint 47</t>
+    <t>TDC Sprint 48</t>
   </si>
   <si>
     <t>TDC-3796</t>
@@ -490,7 +502,7 @@
     <t>TDC-4342</t>
   </si>
   <si>
-    <t>TDC Sprint 48</t>
+    <t>TDC Sprint 49</t>
   </si>
   <si>
     <t>TDC-3951</t>
@@ -526,7 +538,7 @@
     <t>TDC-4519</t>
   </si>
   <si>
-    <t>TDC Sprint 49</t>
+    <t>TDC Sprint 50</t>
   </si>
   <si>
     <t>TDC-4523</t>
@@ -539,18 +551,6 @@
   </si>
   <si>
     <t>TDC-4498</t>
-  </si>
-  <si>
-    <t>TDC Sprint 50</t>
-  </si>
-  <si>
-    <t>2020-08-24T17:30:59.324-05:00</t>
-  </si>
-  <si>
-    <t>2020-09-10T07:54:00.000-05:00</t>
-  </si>
-  <si>
-    <t>2020-09-10T06:31:17.312-05:00</t>
   </si>
   <si>
     <t>TDC-3834</t>
@@ -3400,7 +3400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -3495,43 +3495,58 @@
       <c r="AV3">
         <v>25</v>
       </c>
+      <c r="AW3">
+        <v>1567</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -3558,10 +3573,10 @@
         <v>7.077928240740741</v>
       </c>
       <c r="AJ4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AK4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AL4">
         <v>1.99</v>
@@ -3597,44 +3612,53 @@
         <v>12</v>
       </c>
       <c r="AW4">
-        <v>1567</v>
+        <v>1569</v>
       </c>
       <c r="AX4" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -3665,10 +3689,10 @@
         <v>1.9784027777777777</v>
       </c>
       <c r="AJ5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AK5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AL5">
         <v>0.38</v>
@@ -3704,32 +3728,41 @@
         <v>6</v>
       </c>
       <c r="AW5">
-        <v>1569</v>
+        <v>1617</v>
       </c>
       <c r="AX5" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3752,10 +3785,10 @@
         <v>0</v>
       </c>
       <c r="AJ6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="AK6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AL6">
         <v>12.05</v>
@@ -3791,44 +3824,53 @@
         <v>5</v>
       </c>
       <c r="AW6">
-        <v>1617</v>
+        <v>1656</v>
       </c>
       <c r="AX6" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -3859,10 +3901,10 @@
         <v>5.342604166666668</v>
       </c>
       <c r="AJ7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="AK7" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AL7">
         <v>23.74</v>
@@ -3898,51 +3940,60 @@
         <v>6</v>
       </c>
       <c r="AW7">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="AX7" t="s">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -3981,10 +4032,10 @@
         <v>8.135405092592594</v>
       </c>
       <c r="AJ8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="AK8" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="AL8">
         <v>9.92</v>
@@ -4020,30 +4071,39 @@
         <v>4</v>
       </c>
       <c r="AW8">
-        <v>1657</v>
+        <v>1682</v>
       </c>
       <c r="AX8" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -4068,10 +4128,10 @@
         <v>0</v>
       </c>
       <c r="AJ9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AK9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AL9">
         <v>17.28</v>
@@ -4107,49 +4167,58 @@
         <v>7</v>
       </c>
       <c r="AW9">
-        <v>1682</v>
+        <v>1713</v>
       </c>
       <c r="AX9" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -4185,10 +4254,10 @@
         <v>8.501493055555557</v>
       </c>
       <c r="AJ10" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="AK10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AL10">
         <v>1.21</v>
@@ -4224,56 +4293,65 @@
         <v>6</v>
       </c>
       <c r="AW10">
-        <v>1713</v>
+        <v>1738</v>
       </c>
       <c r="AX10" t="s">
-        <v>144</v>
+        <v>148</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -4312,10 +4390,10 @@
         <v>7.405104166666667</v>
       </c>
       <c r="AJ11" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="AK11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AL11">
         <v>3.15</v>
@@ -4351,49 +4429,58 @@
         <v>3</v>
       </c>
       <c r="AW11">
-        <v>1738</v>
+        <v>1762</v>
       </c>
       <c r="AX11" t="s">
-        <v>159</v>
+        <v>163</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -4429,10 +4516,10 @@
         <v>27.956076388888892</v>
       </c>
       <c r="AJ12" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="AK12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AL12">
         <v>3.28</v>
@@ -4468,30 +4555,39 @@
         <v>6</v>
       </c>
       <c r="AW12">
-        <v>1762</v>
+        <v>1772</v>
       </c>
       <c r="AX12" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -4516,10 +4612,10 @@
         <v>0</v>
       </c>
       <c r="AJ13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="AK13" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AL13">
         <v>3.23</v>
@@ -4554,23 +4650,8 @@
       <c r="AV13">
         <v>2</v>
       </c>
-      <c r="AW13">
-        <v>1772</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>176</v>
-      </c>
-      <c r="AY13" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ13" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA13" t="s">
-        <v>179</v>
-      </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>180</v>
       </c>
@@ -4640,7 +4721,7 @@
         <v>190</v>
       </c>
       <c r="AK14" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AL14">
         <v>1.01</v>
@@ -4670,12 +4751,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
         <v>192</v>
@@ -4684,7 +4765,7 @@
         <v>193</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>194</v>
@@ -4745,7 +4826,7 @@
         <v>201</v>
       </c>
       <c r="AK15" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AL15">
         <v>9.84</v>
@@ -4775,18 +4856,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
         <v>202</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>68</v>
@@ -4835,7 +4916,7 @@
         <v>207</v>
       </c>
       <c r="AK16" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AL16">
         <v>28.05</v>
@@ -4865,12 +4946,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
         <v>209</v>
@@ -4927,10 +5008,10 @@
         <v>5.939965277777778</v>
       </c>
       <c r="AJ17" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="AK17" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL17">
         <v>27.96</v>
@@ -4960,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>217</v>
       </c>
@@ -5035,7 +5116,7 @@
         <v>191</v>
       </c>
       <c r="AK18" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL18">
         <v>13.07</v>
@@ -5065,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>228</v>
       </c>
@@ -5079,7 +5160,7 @@
         <v>219</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>230</v>
@@ -5135,7 +5216,7 @@
         <v>236</v>
       </c>
       <c r="AK19" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL19">
         <v>26.02</v>
@@ -5165,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>237</v>
       </c>
@@ -5230,7 +5311,7 @@
         <v>246</v>
       </c>
       <c r="AK20" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL20">
         <v>11.06</v>
@@ -5260,12 +5341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C21" t="s">
         <v>248</v>
@@ -5274,7 +5355,7 @@
         <v>239</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>249</v>
@@ -5335,7 +5416,7 @@
         <v>256</v>
       </c>
       <c r="AK21" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL21">
         <v>0.73</v>
@@ -5365,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>257</v>
       </c>
@@ -5420,7 +5501,7 @@
         <v>263</v>
       </c>
       <c r="AK22" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL22">
         <v>3.97</v>
@@ -5444,12 +5525,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>264</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C23" t="s">
         <v>265</v>
@@ -5524,7 +5605,7 @@
         <v>275</v>
       </c>
       <c r="AK23" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL23">
         <v>7.67</v>
@@ -5548,7 +5629,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>276</v>
       </c>
@@ -5628,7 +5709,7 @@
         <v>286</v>
       </c>
       <c r="AK24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AL24">
         <v>0.1</v>
@@ -5652,7 +5733,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>201</v>
       </c>
@@ -5666,7 +5747,7 @@
         <v>239</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>288</v>
@@ -5751,9 +5832,9 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
@@ -5765,7 +5846,7 @@
         <v>298</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>299</v>
@@ -5855,7 +5936,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>308</v>
       </c>
@@ -5949,12 +6030,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
         <v>317</v>
@@ -5963,7 +6044,7 @@
         <v>318</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>319</v>
@@ -6058,12 +6139,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>329</v>
@@ -6072,7 +6153,7 @@
         <v>298</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>330</v>
@@ -6157,18 +6238,18 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>338</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
         <v>339</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>259</v>
@@ -6246,12 +6327,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>346</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
         <v>347</v>
@@ -6345,9 +6426,9 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
@@ -6359,7 +6440,7 @@
         <v>359</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>360</v>
@@ -6439,9 +6520,9 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
@@ -6453,7 +6534,7 @@
         <v>368</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>369</v>
@@ -6533,9 +6614,9 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
@@ -6547,7 +6628,7 @@
         <v>219</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>377</v>
@@ -6627,9 +6708,9 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
@@ -6641,7 +6722,7 @@
         <v>384</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>385</v>
@@ -6711,7 +6792,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>207</v>
       </c>
@@ -6725,7 +6806,7 @@
         <v>391</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>392</v>
@@ -6810,12 +6891,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>401</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
         <v>402</v>
@@ -6899,12 +6980,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>411</v>
       </c>
       <c r="B38" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C38" t="s">
         <v>412</v>
@@ -6993,7 +7074,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>420</v>
       </c>
@@ -7067,7 +7148,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>425</v>
       </c>
@@ -7081,7 +7162,7 @@
         <v>427</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>428</v>
@@ -7136,7 +7217,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -7147,7 +7228,7 @@
         <v>430</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>183</v>
@@ -7230,7 +7311,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>356</v>
       </c>
@@ -7312,10 +7393,10 @@
         <v>11.342962962962963</v>
       </c>
       <c r="AJ42" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AK42" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AL42">
         <v>7.08</v>
@@ -7339,7 +7420,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>449</v>
       </c>
@@ -7353,7 +7434,7 @@
         <v>259</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>451</v>
@@ -7401,10 +7482,10 @@
         <v>0.0001736111111111111</v>
       </c>
       <c r="AJ43" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AK43" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AL43">
         <v>1.98</v>
@@ -7428,7 +7509,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>456</v>
       </c>
@@ -7522,12 +7603,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>468</v>
       </c>
       <c r="B45" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
         <v>469</v>
@@ -7626,12 +7707,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>236</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
         <v>480</v>
@@ -7640,7 +7721,7 @@
         <v>481</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>482</v>
@@ -7698,10 +7779,10 @@
         <v>26.016331018518517</v>
       </c>
       <c r="AJ46" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AK46" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL46">
         <v>5.34</v>
@@ -7725,12 +7806,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>316</v>
       </c>
       <c r="B47" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C47" t="s">
         <v>489</v>
@@ -7810,7 +7891,7 @@
         <v>247</v>
       </c>
       <c r="AK47" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL47">
         <v>13.32</v>
@@ -7834,12 +7915,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>500</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C48" t="s">
         <v>501</v>
@@ -7899,7 +7980,7 @@
         <v>507</v>
       </c>
       <c r="AK48" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL48">
         <v>12.03</v>
@@ -7923,12 +8004,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>399</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
         <v>508</v>
@@ -7988,7 +8069,7 @@
         <v>514</v>
       </c>
       <c r="AK49" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL49">
         <v>15.49</v>
@@ -8012,12 +8093,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>246</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
         <v>515</v>
@@ -8026,7 +8107,7 @@
         <v>219</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>516</v>
@@ -8087,7 +8168,7 @@
         <v>523</v>
       </c>
       <c r="AK50" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AL50">
         <v>1.29</v>
@@ -8111,21 +8192,21 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>507</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C51" t="s">
         <v>524</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>525</v>
@@ -8215,12 +8296,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>389</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
         <v>533</v>
@@ -8309,12 +8390,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>540</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C53" t="s">
         <v>541</v>
@@ -8408,18 +8489,18 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>549</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
         <v>550</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>458</v>
@@ -8512,7 +8593,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>559</v>
       </c>
@@ -8601,12 +8682,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>567</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C56" t="s">
         <v>568</v>
@@ -8615,7 +8696,7 @@
         <v>259</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>569</v>
@@ -8690,12 +8771,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="57" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>575</v>
       </c>
       <c r="B57" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
         <v>576</v>
@@ -8789,7 +8870,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>585</v>
       </c>
@@ -8800,7 +8881,7 @@
         <v>586</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>459</v>
@@ -8878,12 +8959,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>328</v>
       </c>
       <c r="B59" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
         <v>593</v>
@@ -8958,7 +9039,7 @@
         <v>228</v>
       </c>
       <c r="AK59" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AL59">
         <v>15.95</v>
@@ -8982,12 +9063,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="60" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>337</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
         <v>602</v>
@@ -9062,7 +9143,7 @@
         <v>611</v>
       </c>
       <c r="AK60" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AL60">
         <v>6.02</v>
@@ -9086,12 +9167,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>612</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C61" t="s">
         <v>613</v>
@@ -9100,7 +9181,7 @@
         <v>211</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>614</v>
@@ -9180,7 +9261,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>429</v>
       </c>
@@ -9274,7 +9355,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>627</v>
       </c>
@@ -9353,7 +9434,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="64" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -9364,7 +9445,7 @@
         <v>633</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>296</v>
@@ -9410,10 +9491,10 @@
         <v>2.0066319444444445</v>
       </c>
       <c r="AJ64" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AK64" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AL64">
         <v>8.14</v>
@@ -9437,7 +9518,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="65" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>638</v>
       </c>
@@ -9489,10 +9570,10 @@
         <v>0</v>
       </c>
       <c r="AJ65" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="AK65" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AL65">
         <v>7.41</v>
@@ -9516,7 +9597,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="66" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>643</v>
       </c>
@@ -9527,10 +9608,10 @@
         <v>633</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>644</v>
@@ -9581,7 +9662,7 @@
         <v>649</v>
       </c>
       <c r="AK66" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AL66">
         <v>15.82</v>
@@ -9605,7 +9686,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="67" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>466</v>
       </c>
@@ -9616,7 +9697,7 @@
         <v>650</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>467</v>
@@ -9685,7 +9766,7 @@
         <v>659</v>
       </c>
       <c r="AK67" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AL67">
         <v>1.36</v>
@@ -9709,7 +9790,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="68" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>660</v>
       </c>
@@ -9759,7 +9840,7 @@
         <v>665</v>
       </c>
       <c r="AK68" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AL68">
         <v>8.94</v>
@@ -9783,12 +9864,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="69" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>666</v>
       </c>
       <c r="B69" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C69" t="s">
         <v>667</v>
@@ -9838,7 +9919,7 @@
         <v>673</v>
       </c>
       <c r="AK69" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AL69">
         <v>1.61</v>
@@ -9862,7 +9943,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="70" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>514</v>
       </c>
@@ -9876,7 +9957,7 @@
         <v>298</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>675</v>
@@ -9961,7 +10042,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="71" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>682</v>
       </c>
@@ -9972,10 +10053,10 @@
         <v>683</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>684</v>
@@ -10045,21 +10126,21 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="72" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>256</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C72" t="s">
         <v>688</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>689</v>
@@ -10144,12 +10225,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="73" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>566</v>
       </c>
       <c r="B73" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C73" t="s">
         <v>696</v>
@@ -10243,7 +10324,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="74" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>611</v>
       </c>
@@ -10257,7 +10338,7 @@
         <v>706</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>707</v>
@@ -10332,12 +10413,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="75" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>649</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
         <v>713</v>
@@ -10346,7 +10427,7 @@
         <v>348</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>714</v>
@@ -10431,12 +10512,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="76" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>722</v>
       </c>
       <c r="B76" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C76" t="s">
         <v>723</v>
@@ -10525,12 +10606,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="77" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>731</v>
       </c>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C77" t="s">
         <v>732</v>
@@ -10599,7 +10680,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="78" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>263</v>
       </c>
@@ -10610,10 +10691,10 @@
         <v>736</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>737</v>
@@ -10693,7 +10774,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="79" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>275</v>
       </c>
@@ -10704,10 +10785,10 @@
         <v>743</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>744</v>
@@ -10787,7 +10868,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="80" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>286</v>
       </c>
@@ -10798,10 +10879,10 @@
         <v>750</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>751</v>
@@ -10881,7 +10962,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="81" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>410</v>
       </c>
@@ -10948,10 +11029,10 @@
         <v>4.040729166666667</v>
       </c>
       <c r="AJ81" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="AK81" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AL81">
         <v>8.5</v>
@@ -10975,7 +11056,7 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="82" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>659</v>
       </c>
@@ -10989,7 +11070,7 @@
         <v>765</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>766</v>
@@ -11045,7 +11126,7 @@
         <v>567</v>
       </c>
       <c r="AK82" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AL82">
         <v>9.97</v>
@@ -11069,12 +11150,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="83" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>437</v>
       </c>
       <c r="B83" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C83" t="s">
         <v>772</v>
@@ -11129,7 +11210,7 @@
         <v>612</v>
       </c>
       <c r="AK83" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AL83">
         <v>5.39</v>
@@ -11153,12 +11234,12 @@
         <v>46.15642476851851</v>
       </c>
     </row>
-    <row r="84" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
         <v>777</v>
@@ -11167,7 +11248,7 @@
         <v>318</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>778</v>
@@ -11220,7 +11301,7 @@
         <v>3.145115740740741</v>
       </c>
     </row>
-    <row r="85" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>712</v>
       </c>
@@ -11282,21 +11363,21 @@
         <v>3.7902199074074074</v>
       </c>
     </row>
-    <row r="86" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C86" t="s">
         <v>790</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>791</v>
@@ -11354,12 +11435,12 @@
         <v>3.275324074074074</v>
       </c>
     </row>
-    <row r="87" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B87" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C87" t="s">
         <v>798</v>
@@ -11368,7 +11449,7 @@
         <v>68</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>799</v>
@@ -11421,12 +11502,12 @@
         <v>3.225173611111111</v>
       </c>
     </row>
-    <row r="88" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>190</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C88" t="s">
         <v>805</v>
@@ -11435,7 +11516,7 @@
         <v>359</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>806</v>
@@ -11493,7 +11574,7 @@
         <v>1.0134606481481483</v>
       </c>
     </row>
-    <row r="89" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>813</v>
       </c>
@@ -11504,10 +11585,10 @@
         <v>814</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>815</v>
@@ -11535,18 +11616,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>345</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C90" t="s">
         <v>816</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>183</v>
@@ -11607,18 +11688,18 @@
         <v>1.3085185185185184</v>
       </c>
     </row>
-    <row r="91" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>366</v>
       </c>
       <c r="B91" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
         <v>824</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>357</v>
@@ -11679,7 +11760,7 @@
         <v>1.888125</v>
       </c>
     </row>
-    <row r="92" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>375</v>
       </c>
@@ -11746,7 +11827,7 @@
         <v>2.079340277777778</v>
       </c>
     </row>
-    <row r="93" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>479</v>
       </c>
@@ -11813,7 +11894,7 @@
         <v>2.860601851851852</v>
       </c>
     </row>
-    <row r="94" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>847</v>
       </c>
@@ -11855,7 +11936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>574</v>
       </c>
@@ -11922,7 +12003,7 @@
         <v>9.023726851851853</v>
       </c>
     </row>
-    <row r="96" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>584</v>
       </c>
@@ -11994,7 +12075,7 @@
         <v>8.829131944444445</v>
       </c>
     </row>
-    <row r="97" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>592</v>
       </c>
@@ -12066,7 +12147,7 @@
         <v>8.828368055555556</v>
       </c>
     </row>
-    <row r="98" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>523</v>
       </c>
@@ -12080,7 +12161,7 @@
         <v>874</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>875</v>
@@ -12133,12 +12214,12 @@
         <v>1.2858101851851853</v>
       </c>
     </row>
-    <row r="99" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>665</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C99" t="s">
         <v>881</v>
@@ -12147,7 +12228,7 @@
         <v>882</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>883</v>
@@ -12205,12 +12286,12 @@
         <v>8.942905092592593</v>
       </c>
     </row>
-    <row r="100" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>721</v>
       </c>
       <c r="B100" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
         <v>890</v>
@@ -12277,7 +12358,7 @@
         <v>9.99767361111111</v>
       </c>
     </row>
-    <row r="101" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>673</v>
       </c>
@@ -12291,7 +12372,7 @@
         <v>765</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>899</v>
@@ -12334,7 +12415,7 @@
         <v>1.6056365740740741</v>
       </c>
     </row>
-    <row r="102" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>730</v>
       </c>
@@ -12345,7 +12426,7 @@
         <v>903</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>458</v>

</xml_diff>